<commit_message>
Add FULLTEXT INDEX for user table
</commit_message>
<xml_diff>
--- a/doc/db/BLOG_TABLE_Design.xlsx
+++ b/doc/db/BLOG_TABLE_Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blog\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blog\doc\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="105">
   <si>
     <t>Table Information</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>FULLTEXT INDEX</t>
+  </si>
+  <si>
+    <t>username, lastname, firstname</t>
   </si>
 </sst>
 </file>
@@ -1072,6 +1078,63 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1098,63 +1161,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1673,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1706,101 +1712,101 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="86"/>
+      <c r="D2" s="73"/>
       <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="87"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="76"/>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="74"/>
+      <c r="G3" s="78"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="74"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="78"/>
     </row>
     <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="73"/>
+      <c r="D5" s="76"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="78"/>
     </row>
     <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="74"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="77"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="81"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="78"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="80"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="80"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="84"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -2172,10 +2178,10 @@
       <c r="B27" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="64"/>
+      <c r="D27" s="83"/>
       <c r="E27" s="39" t="s">
         <v>28</v>
       </c>
@@ -2200,10 +2206,10 @@
       <c r="B28" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="66"/>
+      <c r="D28" s="85"/>
       <c r="E28" s="43" t="s">
         <v>21</v>
       </c>
@@ -2223,9 +2229,13 @@
       <c r="A29" s="45">
         <v>2</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="68"/>
+      <c r="B29" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="87"/>
       <c r="E29" s="46"/>
       <c r="F29" s="46"/>
       <c r="G29" s="47"/>
@@ -2255,14 +2265,14 @@
       <c r="B32" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="69" t="s">
+      <c r="D32" s="89"/>
+      <c r="E32" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="71"/>
+      <c r="F32" s="90"/>
       <c r="G32" s="53" t="s">
         <v>34</v>
       </c>
@@ -2279,14 +2289,14 @@
       <c r="B35" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="69" t="s">
+      <c r="C35" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="70"/>
-      <c r="E35" s="69" t="s">
+      <c r="D35" s="89"/>
+      <c r="E35" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="71"/>
+      <c r="F35" s="90"/>
       <c r="G35" s="53" t="s">
         <v>37</v>
       </c>
@@ -2302,109 +2312,109 @@
       <c r="B41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="85" t="s">
+      <c r="C41" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="86"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="85" t="s">
+      <c r="F41" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="87"/>
+      <c r="G41" s="74"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="72"/>
-      <c r="D42" s="73"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="76"/>
       <c r="E42" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="88" t="s">
+      <c r="F42" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="G42" s="74"/>
+      <c r="G42" s="78"/>
       <c r="M42" s="4"/>
     </row>
     <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="76"/>
       <c r="E43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="72"/>
-      <c r="G43" s="74"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="78"/>
       <c r="M43" s="4"/>
     </row>
     <row r="44" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="72" t="s">
+      <c r="C44" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="73"/>
+      <c r="D44" s="76"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="74"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="78"/>
       <c r="M44" s="4"/>
     </row>
     <row r="45" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="72" t="s">
+      <c r="C45" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="73"/>
+      <c r="D45" s="76"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="74"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="78"/>
       <c r="M45" s="4"/>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="75" t="s">
+      <c r="B46" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="77"/>
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="81"/>
       <c r="M46" s="4"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="78"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="79"/>
-      <c r="E47" s="79"/>
-      <c r="F47" s="79"/>
-      <c r="G47" s="80"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="67"/>
       <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="81"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="80"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="67"/>
       <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="82"/>
-      <c r="C49" s="83"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83"/>
-      <c r="G49" s="84"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="70"/>
+      <c r="G49" s="71"/>
       <c r="M49" s="4"/>
     </row>
     <row r="51" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2659,10 +2669,10 @@
       <c r="B62" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="63" t="s">
+      <c r="C62" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="64"/>
+      <c r="D62" s="83"/>
       <c r="E62" s="39" t="s">
         <v>28</v>
       </c>
@@ -2684,10 +2694,10 @@
       <c r="B63" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="66"/>
+      <c r="D63" s="85"/>
       <c r="E63" s="43" t="s">
         <v>21</v>
       </c>
@@ -2705,8 +2715,8 @@
         <v>2</v>
       </c>
       <c r="B64" s="34"/>
-      <c r="C64" s="67"/>
-      <c r="D64" s="68"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="87"/>
       <c r="E64" s="46"/>
       <c r="F64" s="46"/>
       <c r="G64" s="47"/>
@@ -2733,14 +2743,14 @@
       <c r="B67" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="69" t="s">
+      <c r="C67" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="70"/>
-      <c r="E67" s="69" t="s">
+      <c r="D67" s="89"/>
+      <c r="E67" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="71"/>
+      <c r="F67" s="90"/>
       <c r="G67" s="53" t="s">
         <v>34</v>
       </c>
@@ -2774,14 +2784,14 @@
       <c r="B71" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="69" t="s">
+      <c r="C71" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D71" s="70"/>
-      <c r="E71" s="69" t="s">
+      <c r="D71" s="89"/>
+      <c r="E71" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="F71" s="70"/>
+      <c r="F71" s="89"/>
       <c r="G71" s="53" t="s">
         <v>37</v>
       </c>
@@ -2797,107 +2807,107 @@
       <c r="B77" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="85" t="s">
+      <c r="C77" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="86"/>
+      <c r="D77" s="73"/>
       <c r="E77" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F77" s="85" t="s">
+      <c r="F77" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G77" s="87"/>
+      <c r="G77" s="74"/>
       <c r="M77" s="4"/>
     </row>
     <row r="78" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="73"/>
+      <c r="C78" s="75"/>
+      <c r="D78" s="76"/>
       <c r="E78" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="88" t="s">
+      <c r="F78" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="G78" s="74"/>
+      <c r="G78" s="78"/>
       <c r="M78" s="4"/>
     </row>
     <row r="79" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="72"/>
-      <c r="D79" s="73"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="76"/>
       <c r="E79" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="72"/>
-      <c r="G79" s="74"/>
+      <c r="F79" s="75"/>
+      <c r="G79" s="78"/>
       <c r="M79" s="4"/>
     </row>
     <row r="80" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="C80" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="D80" s="73"/>
+      <c r="D80" s="76"/>
       <c r="E80" s="10"/>
-      <c r="F80" s="72"/>
-      <c r="G80" s="74"/>
+      <c r="F80" s="75"/>
+      <c r="G80" s="78"/>
       <c r="M80" s="4"/>
     </row>
     <row r="81" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="72" t="s">
+      <c r="C81" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D81" s="73"/>
+      <c r="D81" s="76"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="72"/>
-      <c r="G81" s="74"/>
+      <c r="F81" s="75"/>
+      <c r="G81" s="78"/>
       <c r="M81" s="4"/>
     </row>
     <row r="82" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B82" s="75" t="s">
+      <c r="B82" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C82" s="76"/>
-      <c r="D82" s="76"/>
-      <c r="E82" s="76"/>
-      <c r="F82" s="76"/>
-      <c r="G82" s="77"/>
+      <c r="C82" s="80"/>
+      <c r="D82" s="80"/>
+      <c r="E82" s="80"/>
+      <c r="F82" s="80"/>
+      <c r="G82" s="81"/>
       <c r="M82" s="4"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="78"/>
-      <c r="C83" s="79"/>
-      <c r="D83" s="79"/>
-      <c r="E83" s="79"/>
-      <c r="F83" s="79"/>
-      <c r="G83" s="80"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="66"/>
+      <c r="F83" s="66"/>
+      <c r="G83" s="67"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="81"/>
-      <c r="C84" s="79"/>
-      <c r="D84" s="79"/>
-      <c r="E84" s="79"/>
-      <c r="F84" s="79"/>
-      <c r="G84" s="80"/>
+      <c r="B84" s="68"/>
+      <c r="C84" s="66"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="67"/>
     </row>
     <row r="85" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="82"/>
-      <c r="C85" s="83"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="83"/>
-      <c r="F85" s="83"/>
-      <c r="G85" s="84"/>
+      <c r="B85" s="69"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="70"/>
+      <c r="E85" s="70"/>
+      <c r="F85" s="70"/>
+      <c r="G85" s="71"/>
     </row>
     <row r="87" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
@@ -3112,10 +3122,10 @@
       <c r="B97" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C97" s="63" t="s">
+      <c r="C97" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="D97" s="64"/>
+      <c r="D97" s="83"/>
       <c r="E97" s="39" t="s">
         <v>28</v>
       </c>
@@ -3133,10 +3143,10 @@
       <c r="B98" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="65" t="s">
+      <c r="C98" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="D98" s="66"/>
+      <c r="D98" s="85"/>
       <c r="E98" s="43" t="s">
         <v>21</v>
       </c>
@@ -3150,8 +3160,8 @@
         <v>2</v>
       </c>
       <c r="B99" s="34"/>
-      <c r="C99" s="67"/>
-      <c r="D99" s="68"/>
+      <c r="C99" s="86"/>
+      <c r="D99" s="87"/>
       <c r="E99" s="46"/>
       <c r="F99" s="46"/>
       <c r="G99" s="47"/>
@@ -3170,14 +3180,14 @@
       <c r="B102" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="69" t="s">
+      <c r="C102" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D102" s="70"/>
-      <c r="E102" s="69" t="s">
+      <c r="D102" s="89"/>
+      <c r="E102" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="F102" s="71"/>
+      <c r="F102" s="90"/>
       <c r="G102" s="53" t="s">
         <v>34</v>
       </c>
@@ -3226,14 +3236,14 @@
       <c r="B106" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C106" s="69" t="s">
+      <c r="C106" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D106" s="70"/>
-      <c r="E106" s="69" t="s">
+      <c r="D106" s="89"/>
+      <c r="E106" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="F106" s="70"/>
+      <c r="F106" s="89"/>
       <c r="G106" s="53" t="s">
         <v>37</v>
       </c>
@@ -3241,10 +3251,10 @@
     </row>
     <row r="118" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B118" s="4"/>
-      <c r="C118" s="90" t="s">
+      <c r="C118" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="F118" s="89" t="s">
+      <c r="F118" s="63" t="s">
         <v>102</v>
       </c>
       <c r="G118" s="4"/>
@@ -3342,7 +3352,7 @@
     </row>
     <row r="130" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B130" s="4"/>
-      <c r="D130" s="89" t="s">
+      <c r="D130" s="63" t="s">
         <v>100</v>
       </c>
       <c r="G130" s="4"/>
@@ -3427,50 +3437,6 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G49"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="F79:G79"/>
     <mergeCell ref="C106:D106"/>
     <mergeCell ref="E106:F106"/>
     <mergeCell ref="C80:D80"/>
@@ -3484,6 +3450,50 @@
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="E102:F102"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L14" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit table design on delete cascade
</commit_message>
<xml_diff>
--- a/doc/db/BLOG_TABLE_Design.xlsx
+++ b/doc/db/BLOG_TABLE_Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\blog\doc\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\_blog\blog\doc\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="106">
   <si>
     <t>Table Information</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>username, lastname, firstname</t>
+  </si>
+  <si>
+    <t>ON DELETE CASCADE</t>
   </si>
 </sst>
 </file>
@@ -1084,6 +1087,30 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1105,36 +1132,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1153,14 +1150,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1679,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1712,101 +1715,101 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="73"/>
+      <c r="D2" s="88"/>
       <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="89"/>
     </row>
     <row r="3" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="78"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="76"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="78"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="78"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="69"/>
     </row>
     <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="76"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="78"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="81"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="72"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="75"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="71"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -2178,10 +2181,10 @@
       <c r="B27" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="83"/>
+      <c r="D27" s="81"/>
       <c r="E27" s="39" t="s">
         <v>28</v>
       </c>
@@ -2206,10 +2209,10 @@
       <c r="B28" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="84" t="s">
+      <c r="C28" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="85"/>
+      <c r="D28" s="83"/>
       <c r="E28" s="43" t="s">
         <v>21</v>
       </c>
@@ -2232,10 +2235,10 @@
       <c r="B29" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="87"/>
+      <c r="D29" s="85"/>
       <c r="E29" s="46"/>
       <c r="F29" s="46"/>
       <c r="G29" s="47"/>
@@ -2265,14 +2268,14 @@
       <c r="B32" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="88" t="s">
+      <c r="C32" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="88" t="s">
+      <c r="D32" s="66"/>
+      <c r="E32" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="90"/>
+      <c r="F32" s="86"/>
       <c r="G32" s="53" t="s">
         <v>34</v>
       </c>
@@ -2289,14 +2292,14 @@
       <c r="B35" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="88" t="s">
+      <c r="D35" s="66"/>
+      <c r="E35" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="90"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="53" t="s">
         <v>37</v>
       </c>
@@ -2312,109 +2315,109 @@
       <c r="B41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="72" t="s">
+      <c r="C41" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="73"/>
+      <c r="D41" s="88"/>
       <c r="E41" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="72" t="s">
+      <c r="F41" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="74"/>
+      <c r="G41" s="89"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="75"/>
-      <c r="D42" s="76"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
       <c r="E42" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="77" t="s">
+      <c r="F42" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="G42" s="78"/>
+      <c r="G42" s="69"/>
       <c r="M42" s="4"/>
     </row>
     <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="76"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="68"/>
       <c r="E43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="75"/>
-      <c r="G43" s="78"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="69"/>
       <c r="M43" s="4"/>
     </row>
     <row r="44" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="75" t="s">
+      <c r="C44" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="76"/>
+      <c r="D44" s="68"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="78"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="69"/>
       <c r="M44" s="4"/>
     </row>
     <row r="45" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="75" t="s">
+      <c r="C45" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="76"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="78"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="69"/>
       <c r="M45" s="4"/>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="79" t="s">
+      <c r="B46" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="81"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="72"/>
       <c r="M46" s="4"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="65"/>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="66"/>
-      <c r="G47" s="67"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="75"/>
       <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="68"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="66"/>
-      <c r="G48" s="67"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="75"/>
       <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="69"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="71"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="79"/>
       <c r="M49" s="4"/>
     </row>
     <row r="51" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2662,17 +2665,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="82" t="s">
+      <c r="C62" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="83"/>
+      <c r="D62" s="81"/>
       <c r="E62" s="39" t="s">
         <v>28</v>
       </c>
@@ -2694,10 +2697,10 @@
       <c r="B63" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="84" t="s">
+      <c r="C63" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="85"/>
+      <c r="D63" s="83"/>
       <c r="E63" s="43" t="s">
         <v>21</v>
       </c>
@@ -2715,8 +2718,8 @@
         <v>2</v>
       </c>
       <c r="B64" s="34"/>
-      <c r="C64" s="86"/>
-      <c r="D64" s="87"/>
+      <c r="C64" s="84"/>
+      <c r="D64" s="85"/>
       <c r="E64" s="46"/>
       <c r="F64" s="46"/>
       <c r="G64" s="47"/>
@@ -2743,14 +2746,14 @@
       <c r="B67" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="88" t="s">
+      <c r="C67" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="89"/>
-      <c r="E67" s="88" t="s">
+      <c r="D67" s="66"/>
+      <c r="E67" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="90"/>
+      <c r="F67" s="86"/>
       <c r="G67" s="53" t="s">
         <v>34</v>
       </c>
@@ -2784,14 +2787,14 @@
       <c r="B71" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="88" t="s">
+      <c r="C71" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D71" s="89"/>
-      <c r="E71" s="88" t="s">
+      <c r="D71" s="66"/>
+      <c r="E71" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="F71" s="89"/>
+      <c r="F71" s="66"/>
       <c r="G71" s="53" t="s">
         <v>37</v>
       </c>
@@ -2807,107 +2810,107 @@
       <c r="B77" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="72" t="s">
+      <c r="C77" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="73"/>
+      <c r="D77" s="88"/>
       <c r="E77" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F77" s="72" t="s">
+      <c r="F77" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="G77" s="74"/>
+      <c r="G77" s="89"/>
       <c r="M77" s="4"/>
     </row>
     <row r="78" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="75"/>
-      <c r="D78" s="76"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F78" s="77" t="s">
+      <c r="F78" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="G78" s="78"/>
+      <c r="G78" s="69"/>
       <c r="M78" s="4"/>
     </row>
     <row r="79" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="75"/>
-      <c r="D79" s="76"/>
+      <c r="C79" s="67"/>
+      <c r="D79" s="68"/>
       <c r="E79" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="75"/>
-      <c r="G79" s="78"/>
+      <c r="F79" s="67"/>
+      <c r="G79" s="69"/>
       <c r="M79" s="4"/>
     </row>
     <row r="80" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="75" t="s">
+      <c r="C80" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="D80" s="76"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="10"/>
-      <c r="F80" s="75"/>
-      <c r="G80" s="78"/>
+      <c r="F80" s="67"/>
+      <c r="G80" s="69"/>
       <c r="M80" s="4"/>
     </row>
     <row r="81" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="75" t="s">
+      <c r="C81" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="D81" s="76"/>
+      <c r="D81" s="68"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="78"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="69"/>
       <c r="M81" s="4"/>
     </row>
     <row r="82" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B82" s="79" t="s">
+      <c r="B82" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
-      <c r="E82" s="80"/>
-      <c r="F82" s="80"/>
-      <c r="G82" s="81"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="71"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="72"/>
       <c r="M82" s="4"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="65"/>
-      <c r="C83" s="66"/>
-      <c r="D83" s="66"/>
-      <c r="E83" s="66"/>
-      <c r="F83" s="66"/>
-      <c r="G83" s="67"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="74"/>
+      <c r="G83" s="75"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="68"/>
-      <c r="C84" s="66"/>
-      <c r="D84" s="66"/>
-      <c r="E84" s="66"/>
-      <c r="F84" s="66"/>
-      <c r="G84" s="67"/>
+      <c r="B84" s="76"/>
+      <c r="C84" s="74"/>
+      <c r="D84" s="74"/>
+      <c r="E84" s="74"/>
+      <c r="F84" s="74"/>
+      <c r="G84" s="75"/>
     </row>
     <row r="85" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="69"/>
-      <c r="C85" s="70"/>
-      <c r="D85" s="70"/>
-      <c r="E85" s="70"/>
-      <c r="F85" s="70"/>
-      <c r="G85" s="71"/>
+      <c r="B85" s="77"/>
+      <c r="C85" s="78"/>
+      <c r="D85" s="78"/>
+      <c r="E85" s="78"/>
+      <c r="F85" s="78"/>
+      <c r="G85" s="79"/>
     </row>
     <row r="87" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
@@ -3108,24 +3111,26 @@
         <v>21</v>
       </c>
       <c r="F94" s="30"/>
-      <c r="G94" s="31"/>
+      <c r="G94" s="31" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="96" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B97" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C97" s="82" t="s">
+      <c r="C97" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="D97" s="83"/>
+      <c r="D97" s="81"/>
       <c r="E97" s="39" t="s">
         <v>28</v>
       </c>
@@ -3143,10 +3148,10 @@
       <c r="B98" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="84" t="s">
+      <c r="C98" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D98" s="85"/>
+      <c r="D98" s="83"/>
       <c r="E98" s="43" t="s">
         <v>21</v>
       </c>
@@ -3160,8 +3165,8 @@
         <v>2</v>
       </c>
       <c r="B99" s="34"/>
-      <c r="C99" s="86"/>
-      <c r="D99" s="87"/>
+      <c r="C99" s="84"/>
+      <c r="D99" s="85"/>
       <c r="E99" s="46"/>
       <c r="F99" s="46"/>
       <c r="G99" s="47"/>
@@ -3180,14 +3185,14 @@
       <c r="B102" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="88" t="s">
+      <c r="C102" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D102" s="89"/>
-      <c r="E102" s="88" t="s">
+      <c r="D102" s="66"/>
+      <c r="E102" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="F102" s="90"/>
+      <c r="F102" s="86"/>
       <c r="G102" s="53" t="s">
         <v>34</v>
       </c>
@@ -3236,14 +3241,14 @@
       <c r="B106" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C106" s="88" t="s">
+      <c r="C106" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D106" s="89"/>
-      <c r="E106" s="88" t="s">
+      <c r="D106" s="66"/>
+      <c r="E106" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="F106" s="89"/>
+      <c r="F106" s="66"/>
       <c r="G106" s="53" t="s">
         <v>37</v>
       </c>
@@ -3437,6 +3442,50 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G49"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="F79:G79"/>
     <mergeCell ref="C106:D106"/>
     <mergeCell ref="E106:F106"/>
     <mergeCell ref="C80:D80"/>
@@ -3450,50 +3499,6 @@
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="E102:F102"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G49"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L14" r:id="rId1"/>

</xml_diff>